<commit_message>
I now understand how the intersection operator works.
</commit_message>
<xml_diff>
--- a/Excel_Challenge_515 - Normalization of Data.xlsx
+++ b/Excel_Challenge_515 - Normalization of Data.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE04991E-2A15-4D0C-8F29-69C9A8B2AD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ACAEE9-D3A7-40EC-9801-C885F6EFE703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$E$2:$F$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$E$2:$F$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$E$2:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -38,8 +42,85 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="5">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="5">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+    <bk>
+      <rc t="2" v="2"/>
+    </bk>
+    <bk>
+      <rc t="2" v="3"/>
+    </bk>
+    <bk>
+      <rc t="2" v="4"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="24">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -117,12 +198,15 @@
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7226436838398337025/</t>
   </si>
+  <si>
+    <t>Understand</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +222,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +250,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,10 +266,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,8 +283,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,6 +481,336 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D975BA5-67BB-096C-6F07-697CB108DA38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6880860" y="8351520"/>
+          <a:ext cx="7947660" cy="4442460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sure, I’d be happy to help!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The formula =@+A5:B7 in Excel involves two key components: the implicit intersection operator (@) and the range (A5:B7).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Implicit Intersection Operator (@)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The @ symbol is used in Excel to indicate implicit intersection. This operator was introduced to handle dynamic arrays and ensure that formulas return a single value when necessary. Implicit intersection logic works as follows1:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If the value is a single item, it returns that item.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If the value is a range, it returns the value from the cell on the same row or column as the formula.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If the value is an array, it picks the top-left value.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Range (A5:B7)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The range A5:B7 refers to the cells from A5 to B7. This range includes all the cells in the rectangle formed by these two corners.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Combining @ and A5:B7</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>When you use =@+A5:B7, Excel evaluates the range A5:B7 and applies the implicit intersection operator. This means it will return the value from the range that intersects with the cell where the formula is entered. For example, if you enter this formula in cell A6, it will return the value in cell A6 from the range A5:B7.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Practical Example</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Let’s say you have the following data in cells A5:B7:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>A5: 10 B5: 20 A6: 30 B6: 40 A7: 50 B7: 60 If you enter =@+A5:B7 in cell A6, it will return 30 because A6 is the intersecting cell within the specified range.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Does this help clarify how the formula works? If you have any more questions or need further examples, feel free to ask!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>33881</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>10164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="A screenshot of a computer&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6510974E-7B89-3D9F-3CB0-8BA55997488A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1668780" y="13350240"/>
+          <a:ext cx="10717121" cy="4582164"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>338638</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>130247</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="A screenshot of a computer&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{988ADFF2-2F25-6FF7-ED96-548BC351F935}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1668780" y="17922240"/>
+          <a:ext cx="10412278" cy="5068007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+  <rv s="0">
+    <v>John</v>
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v/>
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>Linda</v>
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>Susan</v>
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>William</v>
+    <v>2</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="argument" t="s"/>
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,11 +1074,41 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="935" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{74A11CC4-6F41-4861-AD1F-E8BADA7694BA}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -923,4 +1385,1272 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285B1F1E-00C0-414F-B7C4-76A56F6B03ED}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="N1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="str" cm="1">
+        <f t="array" ref="J3:J6">_xlfn.TEXTSPLIT(B3,,CHAR(10))</f>
+        <v>John :	5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Linda :	8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Susan :	2, 14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="str">
+        <v>William : 11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N1" r:id="rId1" xr:uid="{F3AD2CC1-CEAF-4E90-9274-34A3F6D40067}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5ABF7B-983E-4991-BC43-17DFD889CB1C}">
+  <dimension ref="A1:U122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="str" cm="1">
+        <f t="array" ref="I3:N6">_xlfn.TEXTSPLIT(B3, CHAR({9,32,44,58}), CHAR(10))</f>
+        <v>John</v>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v>5</v>
+      </c>
+      <c r="M3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Linda</v>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v>8</v>
+      </c>
+      <c r="M4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v>2</v>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="str">
+        <v>William</v>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <v>11</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f>CHAR(9)</f>
+        <v xml:space="preserve">	</v>
+      </c>
+      <c r="K10" cm="1">
+        <f t="array" ref="K10:K14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I3), _xlpm.x), 3))(--_xlfn.ANCHORARRAY(I3))</f>
+        <v>5</v>
+      </c>
+      <c r="L10" t="str" cm="1">
+        <f t="array" ref="L10:L14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I3), _xlpm.x), 3))(I3:I6)</f>
+        <v>John</v>
+      </c>
+      <c r="M10" t="str" cm="1">
+        <f t="array" ref="M10:M14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I3), _xlpm.x), 3))(_xlfn.SINGLE(+A3:B3))</f>
+        <v>California</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7" t="str">
+        <f>CHAR(32)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c r="L11" t="str">
+        <v>Linda</v>
+      </c>
+      <c r="M11" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="7" t="str">
+        <f>CHAR(44)</f>
+        <v>,</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="M12" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="7" t="str">
+        <f>CHAR(58)</f>
+        <v>:</v>
+      </c>
+      <c r="K13">
+        <v>14</v>
+      </c>
+      <c r="L13" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="M13" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+      <c r="L14" t="str">
+        <v>William</v>
+      </c>
+      <c r="M14" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="e" cm="1" vm="1">
+        <f t="array" ref="I17:N20">IF(--_xlfn.ANCHORARRAY(I3), I3:I6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L17" t="str">
+        <v>John</v>
+      </c>
+      <c r="M17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P17" t="e" cm="1" vm="1">
+        <f t="array" ref="P17:U20">IF(--_xlfn.ANCHORARRAY(I3), _xlfn.SINGLE(+A3:B3))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S17" t="str">
+        <v>California</v>
+      </c>
+      <c r="T17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L18" t="str">
+        <v>Linda</v>
+      </c>
+      <c r="M18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P18" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S18" t="str">
+        <v>California</v>
+      </c>
+      <c r="T18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L19" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="M19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N19" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="P19" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S19" t="str">
+        <v>California</v>
+      </c>
+      <c r="T19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U19" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L20" t="str">
+        <v>William</v>
+      </c>
+      <c r="M20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P20" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S20" t="str">
+        <v>California</v>
+      </c>
+      <c r="T20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" cm="1">
+        <f t="array" ref="B23:D40">_xlfn.DROP(
+    _xlfn._xlws.SORT(
+        _xlfn.REDUCE(
+            0,
+            B3:B7,
+            _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                _xlfn.LET(
+                    _xlpm.t, _xlfn.TEXTSPLIT(_xlpm.v, CHAR({9,32,44,58}), CHAR(10)),
+                    _xlpm.L, _xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlpm.t, _xlpm.x), 3)),
+                    _xlfn.VSTACK(_xlpm.a, _xlfn.HSTACK(_xlpm.L(--_xlpm.t), _xlpm.L(_xlfn.TAKE(_xlpm.t, , 1)), _xlpm.L(_xlfn.SINGLE(+A7:_xlpm.v))))
+                )
+            )
+        )
+    ),
+    1
+)</f>
+        <v>1</v>
+      </c>
+      <c r="C23" t="str">
+        <v>James</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="D24" t="str">
+        <v>California</v>
+      </c>
+      <c r="I24" t="str" cm="1">
+        <f t="array" ref="I24:P26">_xlfn.TEXTSPLIT(B5, CHAR({9,32,44,58}), CHAR(10))</f>
+        <v>David</v>
+      </c>
+      <c r="J24" t="str">
+        <v/>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <v>13</v>
+      </c>
+      <c r="M24" t="str">
+        <v/>
+      </c>
+      <c r="N24" t="str">
+        <v>15</v>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="str">
+        <v>James</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Kansas</v>
+      </c>
+      <c r="I25" t="str">
+        <v>James</v>
+      </c>
+      <c r="J25" t="str">
+        <v/>
+      </c>
+      <c r="K25" t="str">
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <v>10</v>
+      </c>
+      <c r="M25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O25" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P25" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="str">
+        <v>James</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Ohio</v>
+      </c>
+      <c r="I26" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="J26" t="str">
+        <v/>
+      </c>
+      <c r="K26" t="str">
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <v>12</v>
+      </c>
+      <c r="M26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O26" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P26" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="str">
+        <v>John</v>
+      </c>
+      <c r="D27" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="str">
+        <v>James</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29" t="str">
+        <v>James</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Texas</v>
+      </c>
+      <c r="I29" cm="1">
+        <f t="array" ref="I29:I33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(--_xlfn.ANCHORARRAY(I24))</f>
+        <v>13</v>
+      </c>
+      <c r="J29" t="str" cm="1">
+        <f t="array" ref="J29:J33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(I24:I26)</f>
+        <v>David</v>
+      </c>
+      <c r="K29" t="str" cm="1">
+        <f t="array" ref="K29:K33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(_xlfn.SINGLE(+A5:B7))</f>
+        <v>New York</v>
+      </c>
+      <c r="M29" t="str" cm="1">
+        <f t="array" ref="M29:M33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(_xlfn.SINGLE(+A5:B7))</f>
+        <v>New York</v>
+      </c>
+      <c r="O29" t="str" cm="1">
+        <f t="array" ref="O29">_xlfn.SINGLE(+A5:B7)</f>
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Linda</v>
+      </c>
+      <c r="D30" t="str">
+        <v>California</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+      <c r="J30" t="str">
+        <v>David</v>
+      </c>
+      <c r="K30" t="str">
+        <v>New York</v>
+      </c>
+      <c r="M30" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31" t="str">
+        <v>David</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Kansas</v>
+      </c>
+      <c r="I31">
+        <v>16</v>
+      </c>
+      <c r="J31" t="str">
+        <v>David</v>
+      </c>
+      <c r="K31" t="str">
+        <v>New York</v>
+      </c>
+      <c r="M31" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" t="str">
+        <v>James</v>
+      </c>
+      <c r="D32" t="str">
+        <v>New York</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+      <c r="J32" t="str">
+        <v>James</v>
+      </c>
+      <c r="K32" t="str">
+        <v>New York</v>
+      </c>
+      <c r="M32" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33" t="str">
+        <v>William</v>
+      </c>
+      <c r="D33" t="str">
+        <v>California</v>
+      </c>
+      <c r="I33">
+        <v>12</v>
+      </c>
+      <c r="J33" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="K33" t="str">
+        <v>New York</v>
+      </c>
+      <c r="M33" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="D34" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35" t="str">
+        <v>David</v>
+      </c>
+      <c r="D35" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>14</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="D36" t="str">
+        <v>California</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37" t="str">
+        <v>David</v>
+      </c>
+      <c r="D37" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38" t="str">
+        <v>David</v>
+      </c>
+      <c r="D38" t="str">
+        <v>New York</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>17</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Ohio</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>18</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Sarah</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Kansas</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>20</v>
+      </c>
+      <c r="H120" cm="1">
+        <f t="array" ref="H120">_xlfn.SINGLE(+B120:C122)</f>
+        <v>10</v>
+      </c>
+      <c r="I120" cm="1">
+        <f t="array" ref="I120">_xlfn.SINGLE(+C120:D122)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>30</v>
+      </c>
+      <c r="C121">
+        <v>40</v>
+      </c>
+      <c r="F121" cm="1">
+        <f t="array" ref="F121">_xlfn.SINGLE(+B120:C122)</f>
+        <v>10</v>
+      </c>
+      <c r="H121" cm="1">
+        <f t="array" ref="H121">_xlfn.SINGLE(+B121:C123)</f>
+        <v>30</v>
+      </c>
+      <c r="I121" cm="1">
+        <f t="array" ref="I121">_xlfn.SINGLE(+C121:D123)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>50</v>
+      </c>
+      <c r="C122">
+        <v>60</v>
+      </c>
+      <c r="H122" cm="1">
+        <f t="array" ref="H122">_xlfn.SINGLE(+B122:C124)</f>
+        <v>50</v>
+      </c>
+      <c r="I122" cm="1">
+        <f t="array" ref="I122">_xlfn.SINGLE(+C122:D124)</f>
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worked through Bo's Alt
</commit_message>
<xml_diff>
--- a/Excel_Challenge_515 - Normalization of Data.xlsx
+++ b/Excel_Challenge_515 - Normalization of Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A50FF9-B95B-4534-A808-4089A2AFE2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4C8368-4809-47BA-A9D3-8C3E5F473362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -504,13 +504,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
@@ -793,28 +793,28 @@
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
 <rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
   <rv s="0">
+    <v>2</v>
     <v>John</v>
-    <v>2</v>
     <v>5</v>
   </rv>
   <rv s="0">
+    <v>2</v>
     <v/>
-    <v>2</v>
     <v>5</v>
   </rv>
   <rv s="0">
+    <v>2</v>
     <v>Linda</v>
-    <v>2</v>
     <v>5</v>
   </rv>
   <rv s="0">
+    <v>2</v>
     <v>Susan</v>
-    <v>2</v>
     <v>5</v>
   </rv>
   <rv s="0">
+    <v>2</v>
     <v>William</v>
-    <v>2</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -823,8 +823,8 @@
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
 <rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <s t="_error">
+    <k n="errorType" t="i"/>
     <k n="argument" t="s"/>
-    <k n="errorType" t="i"/>
     <k n="subType" t="i"/>
   </s>
 </rvStructures>
@@ -1408,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285B1F1E-00C0-414F-B7C4-76A56F6B03ED}">
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,40 +1799,35 @@
       </c>
     </row>
     <row r="23" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E23" t="str" cm="1">
-        <f t="array" ref="E23:I35">_xlfn.DROP(_xlfn.REDUCE("",B3:B7,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(_xlpm.t,_xlfn.TEXTSPLIT(_xlpm.v,_nDelim,CHAR(10)),_xlfn.VSTACK(_xlpm.a,_xlpm.t)))),1)</f>
-        <v>John</v>
+      <c r="E23" cm="1">
+        <f t="array" ref="E23:G40">_xlfn._xlws.SORT(_xlfn.DROP(_xlfn.REDUCE("",B3:B7,
+             _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                    _xlfn.LET(_xlpm.t,_xlfn.TEXTSPLIT(_xlpm.v, CHAR({9,32,44,58}), CHAR(10)),
+                        _xlpm.L,_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlpm.t, _xlpm.x), 3)),
+                        _xlfn.VSTACK(_xlpm.a,_xlfn.HSTACK(_xlpm.L(--_xlpm.t),_xlpm.L(_xlfn.TAKE(_xlpm.t,,1)),_xlpm.L(_xlfn.TAKE(_xlpm.t,,-1))))
+                       )
+                   )
+             ),1))</f>
+        <v>1</v>
       </c>
       <c r="F23" t="str">
-        <v/>
+        <v>James</v>
       </c>
       <c r="G23" t="str">
-        <v xml:space="preserve">	5</v>
-      </c>
-      <c r="H23" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I23" t="e">
-        <v>#N/A</v>
+        <v>6</v>
       </c>
       <c r="O23" t="str">
         <v>O</v>
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E24" t="str">
-        <v>Linda</v>
+      <c r="E24">
+        <v>2</v>
       </c>
       <c r="F24" t="str">
-        <v/>
-      </c>
-      <c r="G24" t="str">
-        <v xml:space="preserve">	8</v>
-      </c>
-      <c r="H24" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I24" t="e">
+        <v>Susan</v>
+      </c>
+      <c r="G24" t="e">
         <v>#N/A</v>
       </c>
       <c r="O24" t="str">
@@ -1840,159 +1835,111 @@
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E25" t="str">
-        <v>Susan</v>
+      <c r="E25">
+        <v>3</v>
       </c>
       <c r="F25" t="str">
-        <v/>
+        <v>James</v>
       </c>
       <c r="G25" t="str">
-        <v xml:space="preserve">	2</v>
-      </c>
-      <c r="H25" t="str">
-        <v>14</v>
-      </c>
-      <c r="I25" t="e">
-        <v>#N/A</v>
+        <v>6</v>
       </c>
       <c r="O25" t="str">
         <v>Q</v>
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E26" t="str">
-        <v>William</v>
+      <c r="E26">
+        <v>4</v>
       </c>
       <c r="F26" t="str">
-        <v/>
+        <v>James</v>
       </c>
       <c r="G26" t="str">
-        <v/>
-      </c>
-      <c r="H26" t="str">
-        <v>11</v>
-      </c>
-      <c r="I26" t="e">
-        <v>#N/A</v>
+        <v>4</v>
       </c>
       <c r="O26" t="str">
         <v>R</v>
       </c>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E27" t="str">
-        <v>David</v>
+      <c r="E27">
+        <v>5</v>
       </c>
       <c r="F27" t="str">
-        <v/>
+        <v>John</v>
       </c>
       <c r="G27" t="str">
-        <v xml:space="preserve">	9</v>
-      </c>
-      <c r="H27" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I27" t="e">
-        <v>#N/A</v>
+        <v>14</v>
       </c>
       <c r="O27" t="str">
         <v>S</v>
       </c>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E28" t="str">
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28" t="str">
         <v>James</v>
       </c>
-      <c r="F28" t="str">
-        <v/>
-      </c>
-      <c r="G28" t="str">
-        <v xml:space="preserve">	1</v>
-      </c>
-      <c r="H28" t="str">
-        <v>3</v>
-      </c>
-      <c r="I28" t="str">
-        <v>6</v>
+      <c r="G28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="O28" t="str">
         <v>T</v>
       </c>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E29" t="str">
-        <v>Sarah</v>
+      <c r="E29">
+        <v>7</v>
       </c>
       <c r="F29" t="str">
-        <v/>
+        <v>James</v>
       </c>
       <c r="G29" t="str">
-        <v xml:space="preserve">	18</v>
-      </c>
-      <c r="H29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I29" t="e">
-        <v>#N/A</v>
+        <v>7</v>
       </c>
       <c r="O29" t="str">
         <v>U</v>
       </c>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E30" t="str">
-        <v>David</v>
+      <c r="E30">
+        <v>8</v>
       </c>
       <c r="F30" t="str">
-        <v/>
+        <v>Linda</v>
       </c>
       <c r="G30" t="str">
-        <v xml:space="preserve">	13</v>
-      </c>
-      <c r="H30" t="str">
-        <v>15</v>
-      </c>
-      <c r="I30" t="str">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O30" t="str">
         <v>V</v>
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E31" t="str">
-        <v>James</v>
+      <c r="E31">
+        <v>9</v>
       </c>
       <c r="F31" t="str">
-        <v/>
+        <v>David</v>
       </c>
       <c r="G31" t="str">
-        <v xml:space="preserve">	10</v>
-      </c>
-      <c r="H31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I31" t="e">
-        <v>#N/A</v>
+        <v>6</v>
       </c>
       <c r="O31" t="str">
         <v>W</v>
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="E32" t="str">
-        <v>Susan</v>
+      <c r="E32">
+        <v>10</v>
       </c>
       <c r="F32" t="str">
-        <v/>
-      </c>
-      <c r="G32" t="str">
-        <v/>
-      </c>
-      <c r="H32" t="str">
-        <v>12</v>
-      </c>
-      <c r="I32" t="e">
+        <v>James</v>
+      </c>
+      <c r="G32" t="e">
         <v>#N/A</v>
       </c>
       <c r="O32" t="str">
@@ -2000,19 +1947,13 @@
       </c>
     </row>
     <row r="33" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E33" t="str">
-        <v>James</v>
+      <c r="E33">
+        <v>11</v>
       </c>
       <c r="F33" t="str">
-        <v/>
-      </c>
-      <c r="G33" t="str">
-        <v xml:space="preserve">	4</v>
-      </c>
-      <c r="H33" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I33" t="e">
+        <v>William</v>
+      </c>
+      <c r="G33" t="e">
         <v>#N/A</v>
       </c>
       <c r="O33" t="str">
@@ -2020,19 +1961,13 @@
       </c>
     </row>
     <row r="34" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E34" t="str">
+      <c r="E34">
+        <v>12</v>
+      </c>
+      <c r="F34" t="str">
         <v>Susan</v>
       </c>
-      <c r="F34" t="str">
-        <v/>
-      </c>
-      <c r="G34" t="str">
-        <v xml:space="preserve">	17</v>
-      </c>
-      <c r="H34" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I34" t="e">
+      <c r="G34" t="e">
         <v>#N/A</v>
       </c>
       <c r="O34" t="str">
@@ -2040,46 +1975,85 @@
       </c>
     </row>
     <row r="35" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E35" t="str">
-        <v>James</v>
+      <c r="E35">
+        <v>13</v>
       </c>
       <c r="F35" t="str">
-        <v/>
+        <v>David</v>
       </c>
       <c r="G35" t="str">
-        <v xml:space="preserve">	7</v>
-      </c>
-      <c r="H35" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I35" t="e">
-        <v>#N/A</v>
+        <v>16</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>14</v>
+      </c>
+      <c r="F36" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="O36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>15</v>
+      </c>
+      <c r="F37" t="str">
+        <v>David</v>
+      </c>
+      <c r="G37" t="str">
+        <v>16</v>
+      </c>
       <c r="O37">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>16</v>
+      </c>
+      <c r="F38" t="str">
+        <v>David</v>
+      </c>
+      <c r="G38" t="str">
+        <v>16</v>
+      </c>
       <c r="O38">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>17</v>
+      </c>
+      <c r="F39" t="str">
+        <v>Susan</v>
+      </c>
+      <c r="G39" t="str">
+        <v>17</v>
+      </c>
       <c r="O39">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>18</v>
+      </c>
+      <c r="F40" t="str">
+        <v>Sarah</v>
+      </c>
+      <c r="G40" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="O40">
         <v>5</v>
       </c>
@@ -2115,10 +2089,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5ABF7B-983E-4991-BC43-17DFD889CB1C}">
-  <dimension ref="A1:U122"/>
+  <dimension ref="A1:V122"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2131,17 +2105,17 @@
     <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2158,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2174,27 +2148,27 @@
       <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="str" cm="1">
-        <f t="array" ref="I3:N6">_xlfn.TEXTSPLIT(B3, CHAR({9,32,44,58}), CHAR(10))</f>
+      <c r="J3" t="str" cm="1">
+        <f t="array" ref="J3:O6">_xlfn.TEXTSPLIT(B3, CHAR({9,32,44,58}), CHAR(10))</f>
         <v>John</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
       </c>
       <c r="K3" t="str">
         <v/>
       </c>
       <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
         <v>5</v>
       </c>
-      <c r="M3" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N3" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2210,26 +2184,26 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <v>Linda</v>
-      </c>
-      <c r="J4" t="str">
-        <v/>
       </c>
       <c r="K4" t="str">
         <v/>
       </c>
       <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
         <v>8</v>
       </c>
-      <c r="M4" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N4" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2245,26 +2219,26 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <v>Susan</v>
-      </c>
-      <c r="J5" t="str">
-        <v/>
       </c>
       <c r="K5" t="str">
         <v/>
       </c>
       <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
         <v>2</v>
       </c>
-      <c r="M5" t="str">
+      <c r="N5" t="str">
         <v/>
       </c>
-      <c r="N5" t="str">
+      <c r="O5" t="str">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2280,26 +2254,26 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <v>William</v>
-      </c>
-      <c r="J6" t="str">
-        <v/>
       </c>
       <c r="K6" t="str">
         <v/>
       </c>
       <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
         <v>11</v>
       </c>
-      <c r="M6" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N6" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2316,7 +2290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D8">
         <v>6</v>
       </c>
@@ -2327,7 +2301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D9">
         <v>7</v>
       </c>
@@ -2337,11 +2311,11 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D10">
         <v>8</v>
       </c>
@@ -2351,24 +2325,24 @@
       <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="7" t="str">
+      <c r="J10" s="7" t="str">
         <f>CHAR(9)</f>
         <v xml:space="preserve">	</v>
       </c>
-      <c r="K10" cm="1">
-        <f t="array" ref="K10:K14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I3), _xlpm.x), 3))(--_xlfn.ANCHORARRAY(I3))</f>
+      <c r="L10" cm="1">
+        <f t="array" ref="L10:L14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J3), _xlpm.x), 3))(--_xlfn.ANCHORARRAY(J3))</f>
         <v>5</v>
       </c>
-      <c r="L10" t="str" cm="1">
-        <f t="array" ref="L10:L14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I3), _xlpm.x), 3))(I3:I6)</f>
+      <c r="M10" t="str" cm="1">
+        <f t="array" ref="M10:M14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J3), _xlpm.x), 3))(J3:J6)</f>
         <v>John</v>
       </c>
-      <c r="M10" t="str" cm="1">
-        <f t="array" ref="M10:M14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I3), _xlpm.x), 3))(_xlfn.SINGLE(+A3:B3))</f>
+      <c r="N10" t="str" cm="1">
+        <f t="array" ref="N10:N14">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J3), _xlpm.x), 3))(_xlfn.SINGLE(+A3:B3))</f>
         <v>California</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>9</v>
       </c>
@@ -2378,21 +2352,21 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="7" t="str">
+      <c r="J11" s="7" t="str">
         <f>CHAR(32)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>8</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <v>Linda</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <v>California</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D12">
         <v>10</v>
       </c>
@@ -2402,21 +2376,21 @@
       <c r="F12" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="7" t="str">
+      <c r="J12" s="7" t="str">
         <f>CHAR(44)</f>
         <v>,</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>2</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <v>Susan</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <v>California</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13">
         <v>11</v>
       </c>
@@ -2426,21 +2400,21 @@
       <c r="F13" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="7" t="str">
+      <c r="J13" s="7" t="str">
         <f>CHAR(58)</f>
         <v>:</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>14</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <v>Susan</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <v>California</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D14">
         <v>12</v>
       </c>
@@ -2450,17 +2424,17 @@
       <c r="F14" t="s">
         <v>11</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>11</v>
       </c>
-      <c r="L14" t="str">
+      <c r="M14" t="str">
         <v>William</v>
       </c>
-      <c r="M14" t="str">
+      <c r="N14" t="str">
         <v>California</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>13</v>
       </c>
@@ -2471,7 +2445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>14</v>
       </c>
@@ -2482,7 +2456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D17">
         <v>15</v>
       </c>
@@ -2492,46 +2466,46 @@
       <c r="F17" t="s">
         <v>11</v>
       </c>
-      <c r="I17" t="e" cm="1" vm="1">
-        <f t="array" ref="I17:N20">IF(--_xlfn.ANCHORARRAY(I3), I3:I6)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J17" t="e" vm="2">
+      <c r="J17" t="e" cm="1" vm="1">
+        <f t="array" ref="J17:O20">IF(--_xlfn.ANCHORARRAY(J3), J3:J6)</f>
         <v>#VALUE!</v>
       </c>
       <c r="K17" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L17" t="str">
+      <c r="L17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M17" t="str">
         <v>John</v>
       </c>
-      <c r="M17" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N17" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P17" t="e" cm="1" vm="1">
-        <f t="array" ref="P17:U20">IF(--_xlfn.ANCHORARRAY(I3), _xlfn.SINGLE(+A3:B3))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q17" t="e" vm="2">
+      <c r="O17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" t="e" cm="1" vm="1">
+        <f t="array" ref="Q17:V20">IF(--_xlfn.ANCHORARRAY(J3), _xlfn.SINGLE(+A3:B3))</f>
         <v>#VALUE!</v>
       </c>
       <c r="R17" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="S17" t="str">
+      <c r="S17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T17" t="str">
         <v>California</v>
       </c>
-      <c r="T17" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="U17" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>16</v>
       </c>
@@ -2541,44 +2515,44 @@
       <c r="F18" t="s">
         <v>11</v>
       </c>
-      <c r="I18" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" t="e" vm="2">
+      <c r="J18" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="K18" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L18" t="str">
+      <c r="L18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M18" t="str">
         <v>Linda</v>
       </c>
-      <c r="M18" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N18" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P18" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q18" t="e" vm="2">
+      <c r="O18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="R18" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="S18" t="str">
+      <c r="S18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T18" t="str">
         <v>California</v>
       </c>
-      <c r="T18" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="U18" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D19">
         <v>17</v>
       </c>
@@ -2588,44 +2562,44 @@
       <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="I19" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J19" t="e" vm="2">
+      <c r="J19" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="K19" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L19" t="str">
+      <c r="L19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M19" t="str">
         <v>Susan</v>
       </c>
-      <c r="M19" t="e" vm="2">
+      <c r="N19" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="N19" t="str">
+      <c r="O19" t="str">
         <v>Susan</v>
       </c>
-      <c r="P19" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q19" t="e" vm="2">
+      <c r="Q19" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="R19" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="S19" t="str">
+      <c r="S19" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T19" t="str">
         <v>California</v>
       </c>
-      <c r="T19" t="e" vm="2">
+      <c r="U19" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="U19" t="str">
+      <c r="V19" t="str">
         <v>California</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="D20">
         <v>18</v>
       </c>
@@ -2635,46 +2609,46 @@
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="I20" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" t="e" vm="2">
+      <c r="J20" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="K20" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L20" t="str">
+      <c r="L20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M20" t="str">
         <v>William</v>
       </c>
-      <c r="M20" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N20" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P20" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q20" t="e" vm="2">
+      <c r="O20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q20" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="R20" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="S20" t="str">
+      <c r="S20" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="T20" t="str">
         <v>California</v>
       </c>
-      <c r="T20" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="U20" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" cm="1">
-        <f t="array" ref="B23:D40">_xlfn.DROP(
+        <f t="array" ref="B23:D40">_xlfn._xlws.SORT(_xlfn.DROP(
     _xlfn._xlws.SORT(
         _xlfn.REDUCE(
             0,
@@ -2689,7 +2663,7 @@
         )
     ),
     1
-)</f>
+))</f>
         <v>1</v>
       </c>
       <c r="C23" t="str">
@@ -2698,8 +2672,18 @@
       <c r="D23" t="str">
         <v>Kansas</v>
       </c>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="F23" t="b" cm="1">
+        <f t="array" ref="F23:H40">B23:D40=D3:F20</f>
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2</v>
       </c>
@@ -2709,33 +2693,42 @@
       <c r="D24" t="str">
         <v>California</v>
       </c>
-      <c r="I24" t="str" cm="1">
-        <f t="array" ref="I24:P26">_xlfn.TEXTSPLIT(B5, CHAR({9,32,44,58}), CHAR(10))</f>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="str" cm="1">
+        <f t="array" ref="J24:Q26">_xlfn.TEXTSPLIT(B5, CHAR({9,32,44,58}), CHAR(10))</f>
         <v>David</v>
-      </c>
-      <c r="J24" t="str">
-        <v/>
       </c>
       <c r="K24" t="str">
         <v/>
       </c>
       <c r="L24" t="str">
+        <v/>
+      </c>
+      <c r="M24" t="str">
         <v>13</v>
       </c>
-      <c r="M24" t="str">
+      <c r="N24" t="str">
         <v/>
       </c>
-      <c r="N24" t="str">
+      <c r="O24" t="str">
         <v>15</v>
       </c>
-      <c r="O24" t="str">
+      <c r="P24" t="str">
         <v/>
       </c>
-      <c r="P24" t="str">
+      <c r="Q24" t="str">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>3</v>
       </c>
@@ -2745,21 +2738,27 @@
       <c r="D25" t="str">
         <v>Kansas</v>
       </c>
-      <c r="I25" t="str">
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="str">
         <v>James</v>
-      </c>
-      <c r="J25" t="str">
-        <v/>
       </c>
       <c r="K25" t="str">
         <v/>
       </c>
       <c r="L25" t="str">
+        <v/>
+      </c>
+      <c r="M25" t="str">
         <v>10</v>
       </c>
-      <c r="M25" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N25" t="e">
         <v>#N/A</v>
       </c>
@@ -2769,8 +2768,11 @@
       <c r="P25" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="Q25" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>4</v>
       </c>
@@ -2780,21 +2782,27 @@
       <c r="D26" t="str">
         <v>Ohio</v>
       </c>
-      <c r="I26" t="str">
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="str">
         <v>Susan</v>
-      </c>
-      <c r="J26" t="str">
-        <v/>
       </c>
       <c r="K26" t="str">
         <v/>
       </c>
       <c r="L26" t="str">
+        <v/>
+      </c>
+      <c r="M26" t="str">
         <v>12</v>
       </c>
-      <c r="M26" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="N26" t="e">
         <v>#N/A</v>
       </c>
@@ -2804,8 +2812,11 @@
       <c r="P26" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="Q26" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>5</v>
       </c>
@@ -2815,8 +2826,17 @@
       <c r="D27" t="str">
         <v>California</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>6</v>
       </c>
@@ -2826,8 +2846,17 @@
       <c r="D28" t="str">
         <v>Kansas</v>
       </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>7</v>
       </c>
@@ -2837,28 +2866,37 @@
       <c r="D29" t="str">
         <v>Texas</v>
       </c>
-      <c r="I29" cm="1">
-        <f t="array" ref="I29:I33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(--_xlfn.ANCHORARRAY(I24))</f>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" cm="1">
+        <f t="array" ref="J29:J33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J24), _xlpm.x), 3))(--_xlfn.ANCHORARRAY(J24))</f>
         <v>13</v>
       </c>
-      <c r="J29" t="str" cm="1">
-        <f t="array" ref="J29:J33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(I24:I26)</f>
+      <c r="K29" t="str" cm="1">
+        <f t="array" ref="K29:K33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J24), _xlpm.x), 3))(J24:J26)</f>
         <v>David</v>
       </c>
-      <c r="K29" t="str" cm="1">
-        <f t="array" ref="K29:K33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(_xlfn.SINGLE(+A5:B7))</f>
+      <c r="L29" t="str" cm="1">
+        <f t="array" ref="L29:L33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J24), _xlpm.x), 3))(_xlfn.SINGLE(+A5:B7))</f>
         <v>New York</v>
       </c>
-      <c r="M29" t="str" cm="1">
-        <f t="array" ref="M29:M33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(I24), _xlpm.x), 3))(_xlfn.SINGLE(+A5:B7))</f>
+      <c r="N29" t="str" cm="1">
+        <f t="array" ref="N29:N33">_xlfn.LAMBDA(_xlpm.x, _xlfn.TOCOL(IF(--_xlfn.ANCHORARRAY(J24), _xlpm.x), 3))(_xlfn.SINGLE(+A5:B7))</f>
         <v>New York</v>
       </c>
-      <c r="O29" t="str" cm="1">
-        <f t="array" ref="O29">_xlfn.SINGLE(+A5:B7)</f>
+      <c r="P29" t="str" cm="1">
+        <f t="array" ref="P29">_xlfn.SINGLE(+A5:B7)</f>
         <v>New York</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>8</v>
       </c>
@@ -2868,20 +2906,29 @@
       <c r="D30" t="str">
         <v>California</v>
       </c>
-      <c r="I30">
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30">
         <v>15</v>
       </c>
-      <c r="J30" t="str">
+      <c r="K30" t="str">
         <v>David</v>
       </c>
-      <c r="K30" t="str">
+      <c r="L30" t="str">
         <v>New York</v>
       </c>
-      <c r="M30" t="str">
+      <c r="N30" t="str">
         <v>New York</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>9</v>
       </c>
@@ -2891,20 +2938,29 @@
       <c r="D31" t="str">
         <v>Kansas</v>
       </c>
-      <c r="I31">
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31">
         <v>16</v>
       </c>
-      <c r="J31" t="str">
+      <c r="K31" t="str">
         <v>David</v>
       </c>
-      <c r="K31" t="str">
+      <c r="L31" t="str">
         <v>New York</v>
       </c>
-      <c r="M31" t="str">
+      <c r="N31" t="str">
         <v>New York</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>10</v>
       </c>
@@ -2914,20 +2970,29 @@
       <c r="D32" t="str">
         <v>New York</v>
       </c>
-      <c r="I32">
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32">
         <v>10</v>
       </c>
-      <c r="J32" t="str">
+      <c r="K32" t="str">
         <v>James</v>
       </c>
-      <c r="K32" t="str">
+      <c r="L32" t="str">
         <v>New York</v>
       </c>
-      <c r="M32" t="str">
+      <c r="N32" t="str">
         <v>New York</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>11</v>
       </c>
@@ -2937,20 +3002,29 @@
       <c r="D33" t="str">
         <v>California</v>
       </c>
-      <c r="I33">
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33">
         <v>12</v>
       </c>
-      <c r="J33" t="str">
+      <c r="K33" t="str">
         <v>Susan</v>
       </c>
-      <c r="K33" t="str">
+      <c r="L33" t="str">
         <v>New York</v>
       </c>
-      <c r="M33" t="str">
+      <c r="N33" t="str">
         <v>New York</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>12</v>
       </c>
@@ -2960,8 +3034,17 @@
       <c r="D34" t="str">
         <v>New York</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>13</v>
       </c>
@@ -2971,8 +3054,17 @@
       <c r="D35" t="str">
         <v>New York</v>
       </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>14</v>
       </c>
@@ -2982,8 +3074,17 @@
       <c r="D36" t="str">
         <v>California</v>
       </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>15</v>
       </c>
@@ -2993,8 +3094,17 @@
       <c r="D37" t="str">
         <v>New York</v>
       </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>16</v>
       </c>
@@ -3004,8 +3114,17 @@
       <c r="D38" t="str">
         <v>New York</v>
       </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>17</v>
       </c>
@@ -3015,8 +3134,17 @@
       <c r="D39" t="str">
         <v>Ohio</v>
       </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>18</v>
       </c>
@@ -3026,24 +3154,33 @@
       <c r="D40" t="str">
         <v>Kansas</v>
       </c>
-    </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B120">
         <v>10</v>
       </c>
       <c r="C120">
         <v>20</v>
       </c>
-      <c r="H120" cm="1">
-        <f t="array" ref="H120">_xlfn.SINGLE(+B120:C122)</f>
+      <c r="I120" cm="1">
+        <f t="array" ref="I120">_xlfn.SINGLE(+B120:C122)</f>
         <v>10</v>
       </c>
-      <c r="I120" cm="1">
-        <f t="array" ref="I120">_xlfn.SINGLE(+C120:D122)</f>
+      <c r="J120" cm="1">
+        <f t="array" ref="J120">_xlfn.SINGLE(+C120:D122)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>30</v>
       </c>
@@ -3054,28 +3191,28 @@
         <f t="array" ref="F121">_xlfn.SINGLE(+B120:C122)</f>
         <v>10</v>
       </c>
-      <c r="H121" cm="1">
-        <f t="array" ref="H121">_xlfn.SINGLE(+B121:C123)</f>
+      <c r="I121" cm="1">
+        <f t="array" ref="I121">_xlfn.SINGLE(+B121:C123)</f>
         <v>30</v>
       </c>
-      <c r="I121" cm="1">
-        <f t="array" ref="I121">_xlfn.SINGLE(+C121:D123)</f>
+      <c r="J121" cm="1">
+        <f t="array" ref="J121">_xlfn.SINGLE(+C121:D123)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>50</v>
       </c>
       <c r="C122">
         <v>60</v>
       </c>
-      <c r="H122" cm="1">
-        <f t="array" ref="H122">_xlfn.SINGLE(+B122:C124)</f>
+      <c r="I122" cm="1">
+        <f t="array" ref="I122">_xlfn.SINGLE(+B122:C124)</f>
         <v>50</v>
       </c>
-      <c r="I122" cm="1">
-        <f t="array" ref="I122">_xlfn.SINGLE(+C122:D124)</f>
+      <c r="J122" cm="1">
+        <f t="array" ref="J122">_xlfn.SINGLE(+C122:D124)</f>
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I'm done learning on this one
</commit_message>
<xml_diff>
--- a/Excel_Challenge_515 - Normalization of Data.xlsx
+++ b/Excel_Challenge_515 - Normalization of Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF167C5-58C8-408B-BBCA-A45903C75EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BC5871-37F0-4B01-BC66-AE4241C7BBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3236,7 +3236,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>